<commit_message>
Delete editable supplier number, new edit button
</commit_message>
<xml_diff>
--- a/Test Files/default - Alternate Index Table.xlsx
+++ b/Test Files/default - Alternate Index Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Axell\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Project\WCP Research Tool WebApp\Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6F5066-A292-43A6-B000-9D5A57BF39E1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B8D15C-5C1A-4874-AA31-D16B16AEDEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6255" yWindow="7080" windowWidth="13230" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="22365" yWindow="4365" windowWidth="13230" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="12">
   <si>
     <t>Supplier Name</t>
   </si>
@@ -56,57 +56,6 @@
   </si>
   <si>
     <t>normal</t>
-  </si>
-  <si>
-    <t>1 AUD</t>
-  </si>
-  <si>
-    <t>2 AUD</t>
-  </si>
-  <si>
-    <t>3 AUD</t>
-  </si>
-  <si>
-    <t>4 AUD</t>
-  </si>
-  <si>
-    <t>5 AUD</t>
-  </si>
-  <si>
-    <t>6 AUD</t>
-  </si>
-  <si>
-    <t>7 AUD</t>
-  </si>
-  <si>
-    <t>8 AUD</t>
-  </si>
-  <si>
-    <t>9 AUD</t>
-  </si>
-  <si>
-    <t>10 AUD</t>
-  </si>
-  <si>
-    <t>11 AUD</t>
-  </si>
-  <si>
-    <t>12 AUD</t>
-  </si>
-  <si>
-    <t>13 AUD</t>
-  </si>
-  <si>
-    <t>14 AUD</t>
-  </si>
-  <si>
-    <t>15 AUD</t>
-  </si>
-  <si>
-    <t>16 AUD</t>
-  </si>
-  <si>
-    <t>17 AUD</t>
   </si>
 </sst>
 </file>
@@ -493,7 +442,7 @@
   <dimension ref="A1:H18"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -529,8 +478,8 @@
       <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>12</v>
+      <c r="D2">
+        <v>160</v>
       </c>
       <c r="E2" t="s">
         <v>10</v>
@@ -549,8 +498,8 @@
       <c r="C3" t="s">
         <v>3</v>
       </c>
-      <c r="D3" t="s">
-        <v>13</v>
+      <c r="D3">
+        <v>170</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -569,8 +518,8 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
+      <c r="D4">
+        <v>180</v>
       </c>
       <c r="E4" t="s">
         <v>10</v>
@@ -589,8 +538,8 @@
       <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="D5" t="s">
-        <v>15</v>
+      <c r="D5">
+        <v>190</v>
       </c>
       <c r="E5" t="s">
         <v>10</v>
@@ -609,8 +558,8 @@
       <c r="C6" t="s">
         <v>5</v>
       </c>
-      <c r="D6" t="s">
-        <v>16</v>
+      <c r="D6">
+        <v>200</v>
       </c>
       <c r="E6" t="s">
         <v>10</v>
@@ -629,8 +578,8 @@
       <c r="C7" t="s">
         <v>7</v>
       </c>
-      <c r="D7" t="s">
-        <v>17</v>
+      <c r="D7">
+        <v>210</v>
       </c>
       <c r="E7" t="s">
         <v>10</v>
@@ -649,8 +598,8 @@
       <c r="C8" t="s">
         <v>6</v>
       </c>
-      <c r="D8" t="s">
-        <v>18</v>
+      <c r="D8">
+        <v>220</v>
       </c>
       <c r="E8" t="s">
         <v>10</v>
@@ -669,8 +618,8 @@
       <c r="C9" t="s">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>19</v>
+      <c r="D9">
+        <v>230</v>
       </c>
       <c r="E9" t="s">
         <v>10</v>
@@ -689,8 +638,8 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
-        <v>20</v>
+      <c r="D10">
+        <v>240</v>
       </c>
       <c r="E10" t="s">
         <v>11</v>
@@ -709,8 +658,8 @@
       <c r="C11" t="s">
         <v>2</v>
       </c>
-      <c r="D11" t="s">
-        <v>21</v>
+      <c r="D11">
+        <v>250</v>
       </c>
       <c r="E11" t="s">
         <v>11</v>
@@ -729,8 +678,8 @@
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" t="s">
-        <v>22</v>
+      <c r="D12">
+        <v>260</v>
       </c>
       <c r="E12" t="s">
         <v>11</v>
@@ -749,8 +698,8 @@
       <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="D13" t="s">
-        <v>23</v>
+      <c r="D13">
+        <v>270</v>
       </c>
       <c r="E13" t="s">
         <v>11</v>
@@ -769,8 +718,8 @@
       <c r="C14" t="s">
         <v>7</v>
       </c>
-      <c r="D14" t="s">
-        <v>24</v>
+      <c r="D14">
+        <v>280</v>
       </c>
       <c r="E14" t="s">
         <v>11</v>
@@ -789,8 +738,8 @@
       <c r="C15" t="s">
         <v>6</v>
       </c>
-      <c r="D15" t="s">
-        <v>25</v>
+      <c r="D15">
+        <v>290</v>
       </c>
       <c r="E15" t="s">
         <v>11</v>
@@ -809,8 +758,8 @@
       <c r="C16" t="s">
         <v>1</v>
       </c>
-      <c r="D16" t="s">
-        <v>26</v>
+      <c r="D16">
+        <v>300</v>
       </c>
       <c r="E16" t="s">
         <v>11</v>
@@ -829,8 +778,8 @@
       <c r="C17" t="s">
         <v>3</v>
       </c>
-      <c r="D17" t="s">
-        <v>27</v>
+      <c r="D17">
+        <v>310</v>
       </c>
       <c r="E17" t="s">
         <v>11</v>
@@ -849,8 +798,8 @@
       <c r="C18" t="s">
         <v>2</v>
       </c>
-      <c r="D18" t="s">
-        <v>28</v>
+      <c r="D18">
+        <v>320</v>
       </c>
       <c r="E18" t="s">
         <v>11</v>

</xml_diff>

<commit_message>
Add multiple-select library, update dependencies, update edit AltIndex to work properly, implement populating AltIndex
</commit_message>
<xml_diff>
--- a/Test Files/default - Alternate Index Table.xlsx
+++ b/Test Files/default - Alternate Index Table.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Project\WCP Research Tool WebApp\Test Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B8D15C-5C1A-4874-AA31-D16B16AEDEB5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{593F6E25-DEC7-4BDD-856C-805BD2E5EC57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22365" yWindow="4365" windowWidth="13230" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9330" yWindow="4710" windowWidth="13230" windowHeight="15885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
@@ -20,42 +20,144 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="12">
-  <si>
-    <t>Supplier Name</t>
-  </si>
-  <si>
-    <t>qwe</t>
-  </si>
-  <si>
-    <t>asd</t>
-  </si>
-  <si>
-    <t>zxc</t>
-  </si>
-  <si>
-    <t>ert</t>
-  </si>
-  <si>
-    <t>dfg</t>
-  </si>
-  <si>
-    <t>cvb</t>
-  </si>
-  <si>
-    <t>hjk</t>
-  </si>
-  <si>
-    <t>PT</t>
-  </si>
-  <si>
-    <t>ST</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="46">
   <si>
     <t>Good</t>
   </si>
   <si>
     <t>normal</t>
+  </si>
+  <si>
+    <t>AltIndex-A</t>
+  </si>
+  <si>
+    <t>AltIndex-B</t>
+  </si>
+  <si>
+    <t>AltIndex-C</t>
+  </si>
+  <si>
+    <t>AltIndex-D</t>
+  </si>
+  <si>
+    <t>AltIndex-E</t>
+  </si>
+  <si>
+    <t>AltIndex-F</t>
+  </si>
+  <si>
+    <t>AltIndex-G</t>
+  </si>
+  <si>
+    <t>AltIndex-H</t>
+  </si>
+  <si>
+    <t>AltIndex-I</t>
+  </si>
+  <si>
+    <t>AltIndex-J</t>
+  </si>
+  <si>
+    <t>AltIndex-K</t>
+  </si>
+  <si>
+    <t>AltIndex-L</t>
+  </si>
+  <si>
+    <t>AltIndex-M</t>
+  </si>
+  <si>
+    <t>AltIndex-N</t>
+  </si>
+  <si>
+    <t>AltIndex-O</t>
+  </si>
+  <si>
+    <t>AltIndex-P</t>
+  </si>
+  <si>
+    <t>AltIndex-Q</t>
+  </si>
+  <si>
+    <t>AltIndex-R</t>
+  </si>
+  <si>
+    <t>AltIndex-S</t>
+  </si>
+  <si>
+    <t>AltIndex-T</t>
+  </si>
+  <si>
+    <t>AltIndex-U</t>
+  </si>
+  <si>
+    <t>ENGINE</t>
+  </si>
+  <si>
+    <t>ENG</t>
+  </si>
+  <si>
+    <t>R-201-I1-CS1-1E74</t>
+  </si>
+  <si>
+    <t>R-202-I2-Cb1-C652</t>
+  </si>
+  <si>
+    <t>R-203-I3-CS2-E411</t>
+  </si>
+  <si>
+    <t>R-204-I4-Cf1-4EBF</t>
+  </si>
+  <si>
+    <t>R-205-I5-Ce1-3611</t>
+  </si>
+  <si>
+    <t>R-206-I6-CT1-E14F</t>
+  </si>
+  <si>
+    <t>R-207-I7-CE2-25E7</t>
+  </si>
+  <si>
+    <t>R-208-I8-CS1-DDCC</t>
+  </si>
+  <si>
+    <t>R-209-I9-Cb1-DF3B</t>
+  </si>
+  <si>
+    <t>R-210-I10-CS2-83EE</t>
+  </si>
+  <si>
+    <t>R-211-I11-Cf1-F45F</t>
+  </si>
+  <si>
+    <t>R-212-I12-Ce1-D7D8</t>
+  </si>
+  <si>
+    <t>R-213-I13-CT1-CDB0</t>
+  </si>
+  <si>
+    <t>R-214-I14-CE2-13C6</t>
+  </si>
+  <si>
+    <t>R-215-I15-CS1-3796</t>
+  </si>
+  <si>
+    <t>R-216-I16-Cb1-F8D8</t>
+  </si>
+  <si>
+    <t>R-217-I17-CS2-2EAA</t>
+  </si>
+  <si>
+    <t>R-218-I18-Cf1-5EDB</t>
+  </si>
+  <si>
+    <t>R-219-I19-Ce1-06AD</t>
+  </si>
+  <si>
+    <t>R-220-I20-CT1-3609</t>
+  </si>
+  <si>
+    <t>R-221-I21-CE2-7E27</t>
   </si>
 </sst>
 </file>
@@ -439,393 +541,532 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
+      <c r="A1" s="1">
         <v>1</v>
       </c>
+      <c r="B1">
+        <v>2</v>
+      </c>
       <c r="C1" s="1">
+        <v>3</v>
+      </c>
+      <c r="D1">
+        <v>4</v>
+      </c>
+      <c r="E1">
+        <v>5</v>
+      </c>
+      <c r="F1">
+        <v>6</v>
+      </c>
+      <c r="G1">
+        <v>7</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="C2">
+        <v>5</v>
+      </c>
+      <c r="D2">
+        <v>100</v>
+      </c>
+      <c r="E2" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+      <c r="G2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
+      <c r="C3">
+        <v>10</v>
+      </c>
+      <c r="D3">
+        <v>200</v>
+      </c>
+      <c r="E3" t="s">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
+      <c r="C4">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>300</v>
+      </c>
+      <c r="E4" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" t="s">
+        <v>24</v>
+      </c>
+      <c r="G4" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1">
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>100</v>
+      </c>
+      <c r="E5" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>24</v>
+      </c>
+      <c r="G5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2">
-        <v>160</v>
-      </c>
-      <c r="E2" t="s">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>9</v>
-      </c>
-      <c r="G2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B3">
-        <v>2</v>
-      </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3">
-        <v>170</v>
-      </c>
-      <c r="E3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="G3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B4">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4">
-        <v>180</v>
-      </c>
-      <c r="E4" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" t="s">
-        <v>9</v>
-      </c>
-      <c r="G4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B5">
-        <v>4</v>
-      </c>
-      <c r="C5" t="s">
-        <v>4</v>
-      </c>
-      <c r="D5">
-        <v>190</v>
-      </c>
-      <c r="E5" t="s">
-        <v>10</v>
-      </c>
-      <c r="F5" t="s">
-        <v>9</v>
-      </c>
-      <c r="G5" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B6">
-        <v>5</v>
-      </c>
-      <c r="C6" t="s">
-        <v>5</v>
+      <c r="C6">
+        <v>25</v>
       </c>
       <c r="D6">
         <v>200</v>
       </c>
       <c r="E6" t="s">
+        <v>0</v>
+      </c>
+      <c r="F6" t="s">
+        <v>24</v>
+      </c>
+      <c r="G6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7">
+        <v>30</v>
+      </c>
+      <c r="D7">
+        <v>300</v>
+      </c>
+      <c r="E7" t="s">
+        <v>0</v>
+      </c>
+      <c r="F7" t="s">
+        <v>24</v>
+      </c>
+      <c r="G7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8">
+        <v>35</v>
+      </c>
+      <c r="D8">
+        <v>100</v>
+      </c>
+      <c r="E8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F8" t="s">
+        <v>24</v>
+      </c>
+      <c r="G8" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9">
+        <v>40</v>
+      </c>
+      <c r="D9">
+        <v>200</v>
+      </c>
+      <c r="E9" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="F6" t="s">
-        <v>9</v>
-      </c>
-      <c r="G6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B7">
-        <v>6</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-      <c r="D7">
-        <v>210</v>
-      </c>
-      <c r="E7" t="s">
-        <v>10</v>
-      </c>
-      <c r="F7" t="s">
-        <v>9</v>
-      </c>
-      <c r="G7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B8">
-        <v>7</v>
-      </c>
-      <c r="C8" t="s">
-        <v>6</v>
-      </c>
-      <c r="D8">
-        <v>220</v>
-      </c>
-      <c r="E8" t="s">
-        <v>10</v>
-      </c>
-      <c r="F8" t="s">
-        <v>9</v>
-      </c>
-      <c r="G8" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B9">
-        <v>8</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C10">
+        <v>45</v>
+      </c>
+      <c r="D10">
+        <v>300</v>
+      </c>
+      <c r="E10" t="s">
         <v>1</v>
       </c>
-      <c r="D9">
-        <v>230</v>
-      </c>
-      <c r="E9" t="s">
-        <v>10</v>
-      </c>
-      <c r="F9" t="s">
-        <v>9</v>
-      </c>
-      <c r="G9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B10">
-        <v>9</v>
-      </c>
-      <c r="C10" t="s">
-        <v>3</v>
-      </c>
-      <c r="D10">
-        <v>240</v>
-      </c>
-      <c r="E10" t="s">
+      <c r="F10" t="s">
+        <v>24</v>
+      </c>
+      <c r="G10" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" t="s">
         <v>11</v>
       </c>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>10</v>
-      </c>
-      <c r="C11" t="s">
-        <v>2</v>
+      <c r="C11">
+        <v>50</v>
       </c>
       <c r="D11">
-        <v>250</v>
+        <v>100</v>
       </c>
       <c r="E11" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F11" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G11" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>11</v>
-      </c>
-      <c r="C12" t="s">
-        <v>4</v>
+      <c r="A12" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12">
+        <v>55</v>
       </c>
       <c r="D12">
-        <v>260</v>
+        <v>200</v>
       </c>
       <c r="E12" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F12" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>12</v>
-      </c>
-      <c r="C13" t="s">
-        <v>5</v>
+      <c r="A13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13">
+        <v>60</v>
       </c>
       <c r="D13">
-        <v>270</v>
+        <v>300</v>
       </c>
       <c r="E13" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F13" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G13" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>13</v>
-      </c>
-      <c r="C14" t="s">
-        <v>7</v>
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14">
+        <v>65</v>
       </c>
       <c r="D14">
-        <v>280</v>
+        <v>100</v>
       </c>
       <c r="E14" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F14" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G14" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>14</v>
-      </c>
-      <c r="C15" t="s">
-        <v>6</v>
+      <c r="A15" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C15">
+        <v>70</v>
       </c>
       <c r="D15">
-        <v>290</v>
+        <v>200</v>
       </c>
       <c r="E15" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F15" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G15" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B16">
-        <v>15</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" t="s">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>75</v>
       </c>
       <c r="D16">
         <v>300</v>
       </c>
       <c r="E16" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F16" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G16" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17">
-        <v>16</v>
-      </c>
-      <c r="C17" t="s">
-        <v>3</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" t="s">
+        <v>17</v>
+      </c>
+      <c r="C17">
+        <v>80</v>
       </c>
       <c r="D17">
-        <v>310</v>
+        <v>100</v>
       </c>
       <c r="E17" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F17" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G17" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <v>17</v>
-      </c>
-      <c r="C18" t="s">
-        <v>2</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18">
+        <v>85</v>
       </c>
       <c r="D18">
-        <v>320</v>
+        <v>200</v>
       </c>
       <c r="E18" t="s">
-        <v>11</v>
+        <v>1</v>
       </c>
       <c r="F18" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="G18" t="s">
-        <v>8</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19">
+        <v>90</v>
+      </c>
+      <c r="D19">
+        <v>300</v>
+      </c>
+      <c r="E19" t="s">
+        <v>0</v>
+      </c>
+      <c r="F19" t="s">
+        <v>24</v>
+      </c>
+      <c r="G19" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" t="s">
+        <v>20</v>
+      </c>
+      <c r="C20">
+        <v>95</v>
+      </c>
+      <c r="D20">
+        <v>100</v>
+      </c>
+      <c r="E20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>24</v>
+      </c>
+      <c r="G20" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21">
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>200</v>
+      </c>
+      <c r="E21" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" t="s">
+        <v>24</v>
+      </c>
+      <c r="G21" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" t="s">
+        <v>22</v>
+      </c>
+      <c r="C22">
+        <v>105</v>
+      </c>
+      <c r="D22">
+        <v>300</v>
+      </c>
+      <c r="E22" t="s">
+        <v>0</v>
+      </c>
+      <c r="F22" t="s">
+        <v>24</v>
+      </c>
+      <c r="G22" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="F1"/>
-    <mergeCell ref="G1"/>
+  <mergeCells count="3">
     <mergeCell ref="H1"/>
     <mergeCell ref="A1"/>
-    <mergeCell ref="B1"/>
     <mergeCell ref="C1"/>
-    <mergeCell ref="D1"/>
-    <mergeCell ref="E1"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A1 A6:A11 A2 A3 A4 A5 H3 H4 H5 H7 H6 H9:H11 H8" numberStoredAsText="1"/>
+    <ignoredError sqref="H3 H4 H5 H7 H6 H9:H11 H8" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>